<commit_message>
Update diagram and user requirement
</commit_message>
<xml_diff>
--- a/documenation/MODULES/Characters/UI AI.xlsx
+++ b/documenation/MODULES/Characters/UI AI.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Problem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CC42E62-EFF2-45EA-B7FF-7F3029489613}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E1BC798-A584-4AA1-8CF2-198E873498C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{6DE395C4-104E-47B7-8C72-D6787FD0F0E7}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="375">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="373">
   <si>
     <t>Test Case Description</t>
   </si>
@@ -483,69 +483,15 @@
     <t>UR-007</t>
   </si>
   <si>
-    <t>Input/Output</t>
-  </si>
-  <si>
-    <t>Textbox</t>
-  </si>
-  <si>
-    <t>INPUT</t>
-  </si>
-  <si>
-    <t>Textarea</t>
-  </si>
-  <si>
-    <t>File upload</t>
-  </si>
-  <si>
-    <t>Dropdown</t>
-  </si>
-  <si>
-    <t>Button</t>
-  </si>
-  <si>
-    <t>Table</t>
-  </si>
-  <si>
-    <t>OUTPUT</t>
-  </si>
-  <si>
-    <t>Button (icon)</t>
-  </si>
-  <si>
-    <t>Grid selector</t>
-  </si>
-  <si>
     <t>UR-008</t>
   </si>
   <si>
     <t>UR-009</t>
   </si>
   <si>
-    <t>UR-010</t>
-  </si>
-  <si>
-    <t>Initial Value</t>
-  </si>
-  <si>
-    <t>Description (Mapping with DB if applicable)</t>
-  </si>
-  <si>
-    <t>Character Description</t>
-  </si>
-  <si>
-    <t>Character Avatar</t>
-  </si>
-  <si>
-    <t>Language Style</t>
-  </si>
-  <si>
     <t>Create Character</t>
   </si>
   <si>
-    <t>Character List</t>
-  </si>
-  <si>
     <t>Edit Character</t>
   </si>
   <si>
@@ -553,412 +499,6 @@
   </si>
   <si>
     <t>Assign Character to Conversation Flow</t>
-  </si>
-  <si>
-    <t xml:space="preserve">	Assign Character to Conversation Flow</t>
-  </si>
-  <si>
-    <t>Select Character to Start Chat</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Mandatory</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">: User must provide a character name.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Validation:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Minimum 3 characters.
-Should not duplicate existing character names (validated via backend).
-May support real-time validation for uniqueness.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>User Experience:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Shows inline error message if empty or too short.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Backend Interaction:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Sent as part of request payload to POST /api/characters/create or PUT /api/characters/update/{id}.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Database Mapping: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>characters.name</t>
-    </r>
-  </si>
-  <si>
-    <t>Optional, but recommended.
-Should be concise and describe the character’s personality.
-Max Length: 255 characters.
-Appears when selecting a character in chat interface.
-Backend Interaction:
-Included in character creation/update APIs.
-Database Mapping: characters.description</t>
-  </si>
-  <si>
-    <t>Optional: User may skip uploading.
-File Types Supported: .png, .jpg, .jpeg
-Max File Size: (as defined by system; e.g., 2MB)
-UX Notes:
-Preview thumbnail after file is selected.
-Option to remove or replace the image before saving.
-Backend Interaction:
-File uploaded and returned as a URL.
-URL included in POST /api/characters/create or PUT /api/characters/update/{id}
-Database Mapping: characters.avatar_url</t>
-  </si>
-  <si>
-    <t>Requirements:
-Options:
-Formal, Friendly, Humorous, Serious, etc.
-Must choose one style; default is "Neutral".
-Affects chatbot's tone in conversation.
-Backend Interaction:
-Selected value sent in create/update requests.
-Database Mapping: characters.tone_style</t>
-  </si>
-  <si>
-    <t>Action</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Displays all available characters.
-Includes avatar, name, and description.
-On click, save character_id to user session or local state.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Effect:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-This character's tone and style are applied in the chat session.
-No backend call required unless session is saved server-side.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Used to attach a character to a specific conversation flow.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>On Selection:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Trigger API: PATCH /api/conversation-flow/assign-character
-Send: flow_id, character_id
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Post-action:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Confirmation or visual feedback that assignment succeeded.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">On click, show confirmation dialog: “Are you sure you want to delete this character?”
-If confirmed, call DELETE /api/characters/delete/{id}
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Post-action:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-On success, remove character from list.
-Show message: “Character deleted successfully.”</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">On click, open a popup/modal with pre-filled character info.
-Allows editing all fields except ID.
-On submit, send updated data to PUT /api/characters/update/{id}
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Post-action:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-On success, update character list and close modal.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Displays all existing characters.
-Automatically loads on page/component mount.
-Backend Source: GET /api/characters/list
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Columns to Display:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Avatar thumbnail, Name, Description, Language Style, Action buttons (Edit/Delete)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Visible only when required fields (e.g., Name) are filled correctly.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">On Click:
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Triggers form validation.
-If valid, sends data to POST /api/characters/create.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Expected Responses:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Success → Show toast/alert: "Character created successfully".
-Error → Show warnings (e.g., "Character name is required").
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Post-action:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Clear form or redirect to character list.</t>
-    </r>
   </si>
   <si>
     <t>User Req</t>
@@ -1980,6 +1520,93 @@
   </si>
   <si>
     <t>T11</t>
+  </si>
+  <si>
+    <t>Goal (What)</t>
+  </si>
+  <si>
+    <t>Benefit (Why)</t>
+  </si>
+  <si>
+    <t>As a Registered User, I want to create a new character profile</t>
+  </si>
+  <si>
+    <t>Create a new character</t>
+  </si>
+  <si>
+    <t>So I can personalize my chatbot interactions</t>
+  </si>
+  <si>
+    <t>As a Registered User, I want to edit a character’s name and traits</t>
+  </si>
+  <si>
+    <t>Edit character profile</t>
+  </si>
+  <si>
+    <t>So I can update the character to reflect my preferences</t>
+  </si>
+  <si>
+    <t>As a Registered User, I want to delete a character I no longer need</t>
+  </si>
+  <si>
+    <t>Delete unwanted character</t>
+  </si>
+  <si>
+    <t>So my list of characters stays organized and relevant</t>
+  </si>
+  <si>
+    <t>As a Registered User, I want to view a list of all my characters</t>
+  </si>
+  <si>
+    <t>View all characters</t>
+  </si>
+  <si>
+    <t>So I can easily choose the one I want to use</t>
+  </si>
+  <si>
+    <t>As a Registered User, I want to assign a default character for my chats</t>
+  </si>
+  <si>
+    <t>Set default character</t>
+  </si>
+  <si>
+    <t>So my chatbot uses the preferred character automatically</t>
+  </si>
+  <si>
+    <t>As a Registered User, I want to duplicate a character profile</t>
+  </si>
+  <si>
+    <t>Duplicate character</t>
+  </si>
+  <si>
+    <t>So I can create similar characters with slight changes</t>
+  </si>
+  <si>
+    <t>As a Registered User, I want to search characters by name or tag</t>
+  </si>
+  <si>
+    <t>Search character list</t>
+  </si>
+  <si>
+    <t>So I can find specific characters quickly</t>
+  </si>
+  <si>
+    <t>As a Registered User, I want to filter characters by category or use frequency</t>
+  </si>
+  <si>
+    <t>Filter characters</t>
+  </si>
+  <si>
+    <t>So I can better manage my character library</t>
+  </si>
+  <si>
+    <t>As a Registered User, I want to export my characters as a file</t>
+  </si>
+  <si>
+    <t>Export character data</t>
+  </si>
+  <si>
+    <t>So I can back them up or use them elsewhere</t>
   </si>
 </sst>
 </file>
@@ -2261,7 +1888,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2302,9 +1929,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2358,33 +1982,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2394,10 +1991,43 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2752,14 +2382,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="27" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="30"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="29"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
@@ -2767,12 +2397,12 @@
       <c r="L1" s="1"/>
     </row>
     <row r="2" spans="1:12">
-      <c r="A2" s="31"/>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="33"/>
+      <c r="A2" s="30"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="32"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
@@ -2780,14 +2410,14 @@
       <c r="L2" s="1"/>
     </row>
     <row r="3" spans="1:12">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="20"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="21"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="20"/>
       <c r="G3" s="12"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
@@ -2796,12 +2426,12 @@
       <c r="L3" s="1"/>
     </row>
     <row r="4" spans="1:12" ht="15.6">
-      <c r="A4" s="25"/>
-      <c r="B4" s="26"/>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="27"/>
+      <c r="A4" s="24"/>
+      <c r="B4" s="25"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="26"/>
       <c r="G4" s="2" t="s">
         <v>38</v>
       </c>
@@ -3036,14 +2666,14 @@
       <c r="L12" s="1"/>
     </row>
     <row r="13" spans="1:12" ht="15.6">
-      <c r="A13" s="19" t="s">
+      <c r="A13" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="B13" s="20"/>
-      <c r="C13" s="20"/>
-      <c r="D13" s="20"/>
-      <c r="E13" s="20"/>
-      <c r="F13" s="21"/>
+      <c r="B13" s="19"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="20"/>
       <c r="G13" s="3" t="s">
         <v>45</v>
       </c>
@@ -3054,12 +2684,12 @@
       <c r="L13" s="1"/>
     </row>
     <row r="14" spans="1:12" ht="15.6">
-      <c r="A14" s="22"/>
-      <c r="B14" s="23"/>
-      <c r="C14" s="23"/>
-      <c r="D14" s="23"/>
-      <c r="E14" s="23"/>
-      <c r="F14" s="24"/>
+      <c r="A14" s="21"/>
+      <c r="B14" s="22"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="22"/>
+      <c r="E14" s="22"/>
+      <c r="F14" s="23"/>
       <c r="G14" s="3" t="s">
         <v>34</v>
       </c>
@@ -3070,12 +2700,12 @@
       <c r="L14" s="1"/>
     </row>
     <row r="15" spans="1:12" ht="15.6">
-      <c r="A15" s="25"/>
-      <c r="B15" s="26"/>
-      <c r="C15" s="26"/>
-      <c r="D15" s="26"/>
-      <c r="E15" s="26"/>
-      <c r="F15" s="27"/>
+      <c r="A15" s="24"/>
+      <c r="B15" s="25"/>
+      <c r="C15" s="25"/>
+      <c r="D15" s="25"/>
+      <c r="E15" s="25"/>
+      <c r="F15" s="26"/>
       <c r="G15" s="2" t="s">
         <v>41</v>
       </c>
@@ -3261,30 +2891,30 @@
       </c>
     </row>
     <row r="23" spans="1:12">
-      <c r="A23" s="19" t="s">
+      <c r="A23" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="B23" s="20"/>
-      <c r="C23" s="20"/>
-      <c r="D23" s="20"/>
-      <c r="E23" s="20"/>
-      <c r="F23" s="21"/>
+      <c r="B23" s="19"/>
+      <c r="C23" s="19"/>
+      <c r="D23" s="19"/>
+      <c r="E23" s="19"/>
+      <c r="F23" s="20"/>
     </row>
     <row r="24" spans="1:12">
-      <c r="A24" s="22"/>
-      <c r="B24" s="23"/>
-      <c r="C24" s="23"/>
-      <c r="D24" s="23"/>
-      <c r="E24" s="23"/>
-      <c r="F24" s="24"/>
+      <c r="A24" s="21"/>
+      <c r="B24" s="22"/>
+      <c r="C24" s="22"/>
+      <c r="D24" s="22"/>
+      <c r="E24" s="22"/>
+      <c r="F24" s="23"/>
     </row>
     <row r="25" spans="1:12">
-      <c r="A25" s="25"/>
-      <c r="B25" s="26"/>
-      <c r="C25" s="26"/>
-      <c r="D25" s="26"/>
-      <c r="E25" s="26"/>
-      <c r="F25" s="27"/>
+      <c r="A25" s="24"/>
+      <c r="B25" s="25"/>
+      <c r="C25" s="25"/>
+      <c r="D25" s="25"/>
+      <c r="E25" s="25"/>
+      <c r="F25" s="26"/>
     </row>
     <row r="26" spans="1:12">
       <c r="A26" s="6" t="s">
@@ -3495,219 +3125,192 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B3CDB52-8DB2-4C57-ADD1-806C25E0A913}">
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection sqref="A1:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="7.21875" style="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.88671875" style="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11" style="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="128.88671875" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.44140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.33203125" style="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="50.44140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="42.6640625" style="10" customWidth="1"/>
     <col min="6" max="16384" width="8.88671875" style="10"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="34" t="s">
-        <v>178</v>
-      </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
+      <c r="A1" s="48" t="s">
+        <v>147</v>
+      </c>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="47"/>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="34"/>
-      <c r="B2" s="34"/>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
+      <c r="A2" s="48"/>
+      <c r="B2" s="48"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="47"/>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="48"/>
+      <c r="B3" s="48"/>
+      <c r="C3" s="48"/>
+      <c r="D3" s="48"/>
+      <c r="E3" s="11"/>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B4" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C4" s="6" t="s">
+        <v>344</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>345</v>
+      </c>
+      <c r="E4" s="13"/>
+    </row>
+    <row r="5" spans="1:5" ht="28.8">
+      <c r="A5" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>346</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>347</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>348</v>
+      </c>
+      <c r="E5" s="46"/>
+    </row>
+    <row r="6" spans="1:5" ht="28.8">
+      <c r="A6" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>349</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>350</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>351</v>
+      </c>
+      <c r="E6" s="46"/>
+    </row>
+    <row r="7" spans="1:5" ht="28.8">
+      <c r="A7" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>352</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>353</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>354</v>
+      </c>
+      <c r="E7" s="46"/>
+    </row>
+    <row r="8" spans="1:5" ht="28.8">
+      <c r="A8" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>355</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>356</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>357</v>
+      </c>
+      <c r="E8" s="46"/>
+    </row>
+    <row r="9" spans="1:5" ht="28.8">
+      <c r="A9" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>358</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>359</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>360</v>
+      </c>
+      <c r="E9" s="46"/>
+    </row>
+    <row r="10" spans="1:5" ht="28.8">
+      <c r="A10" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>361</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>362</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>363</v>
+      </c>
+      <c r="E10" s="46"/>
+    </row>
+    <row r="11" spans="1:5" ht="28.8">
+      <c r="A11" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>364</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>365</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>366</v>
+      </c>
+      <c r="E11" s="46"/>
+    </row>
+    <row r="12" spans="1:5" ht="28.8">
+      <c r="A12" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="D3" s="11" t="s">
-        <v>155</v>
-      </c>
-      <c r="E3" s="11" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="273.60000000000002">
-      <c r="A4" s="13" t="s">
-        <v>112</v>
-      </c>
-      <c r="C4" s="14" t="s">
+      <c r="B12" s="7" t="s">
+        <v>367</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>368</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>369</v>
+      </c>
+      <c r="E12" s="46"/>
+    </row>
+    <row r="13" spans="1:5" ht="28.8">
+      <c r="A13" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="D4" s="14" t="s">
-        <v>143</v>
-      </c>
-      <c r="E4" s="15" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="187.2">
-      <c r="A5" s="13" t="s">
-        <v>113</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>157</v>
-      </c>
-      <c r="C5" s="14" t="s">
-        <v>144</v>
-      </c>
-      <c r="D5" s="14" t="s">
-        <v>143</v>
-      </c>
-      <c r="E5" s="15" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="273.60000000000002">
-      <c r="A6" s="13" t="s">
-        <v>114</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>158</v>
-      </c>
-      <c r="C6" s="14" t="s">
-        <v>145</v>
-      </c>
-      <c r="D6" s="14" t="s">
-        <v>143</v>
-      </c>
-      <c r="E6" s="15" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="201.6">
-      <c r="A7" s="13" t="s">
-        <v>115</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>159</v>
-      </c>
-      <c r="C7" s="14" t="s">
-        <v>146</v>
-      </c>
-      <c r="D7" s="14" t="s">
-        <v>143</v>
-      </c>
-      <c r="E7" s="15" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="244.8">
-      <c r="A8" s="13" t="s">
-        <v>116</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>160</v>
-      </c>
-      <c r="C8" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="D8" s="14" t="s">
-        <v>171</v>
-      </c>
-      <c r="E8" s="15" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="129.6">
-      <c r="A9" s="13" t="s">
-        <v>139</v>
-      </c>
-      <c r="B9" s="14" t="s">
-        <v>161</v>
-      </c>
-      <c r="C9" s="14" t="s">
-        <v>148</v>
-      </c>
-      <c r="D9" s="14" t="s">
-        <v>149</v>
-      </c>
-      <c r="E9" s="15" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="129.6">
-      <c r="A10" s="13" t="s">
-        <v>140</v>
-      </c>
-      <c r="B10" s="14" t="s">
-        <v>162</v>
-      </c>
-      <c r="C10" s="14" t="s">
-        <v>150</v>
-      </c>
-      <c r="D10" s="14" t="s">
-        <v>171</v>
-      </c>
-      <c r="E10" s="15" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="129.6">
-      <c r="A11" s="13" t="s">
-        <v>152</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>163</v>
-      </c>
-      <c r="C11" s="14" t="s">
-        <v>150</v>
-      </c>
-      <c r="D11" s="14" t="s">
-        <v>171</v>
-      </c>
-      <c r="E11" s="15" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="158.4">
-      <c r="A12" s="13" t="s">
-        <v>153</v>
-      </c>
-      <c r="B12" s="14" t="s">
-        <v>165</v>
-      </c>
-      <c r="C12" s="14" t="s">
-        <v>146</v>
-      </c>
-      <c r="D12" s="14" t="s">
-        <v>143</v>
-      </c>
-      <c r="E12" s="15" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="158.4">
-      <c r="A13" s="13" t="s">
-        <v>154</v>
-      </c>
-      <c r="B13" s="14" t="s">
-        <v>166</v>
-      </c>
-      <c r="C13" s="14" t="s">
-        <v>151</v>
-      </c>
-      <c r="D13" s="14" t="s">
-        <v>143</v>
-      </c>
-      <c r="E13" s="15" t="s">
-        <v>172</v>
-      </c>
+      <c r="B13" s="7" t="s">
+        <v>370</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>371</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>372</v>
+      </c>
+      <c r="E13" s="46"/>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="13"/>
@@ -3772,7 +3375,7 @@
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:E2"/>
+    <mergeCell ref="A1:D3"/>
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3799,816 +3402,762 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="40.049999999999997" customHeight="1">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="33" t="s">
         <v>117</v>
       </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="45"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="35"/>
     </row>
     <row r="2" spans="1:13" ht="40.049999999999997" customHeight="1">
-      <c r="A2" s="42" t="s">
-        <v>179</v>
-      </c>
-      <c r="B2" s="42"/>
-      <c r="C2" s="42"/>
-      <c r="D2" s="42"/>
-      <c r="E2" s="42"/>
-      <c r="F2" s="42"/>
+      <c r="A2" s="40" t="s">
+        <v>148</v>
+      </c>
+      <c r="B2" s="40"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
     </row>
     <row r="3" spans="1:13" ht="40.049999999999997" customHeight="1">
-      <c r="A3" s="42"/>
-      <c r="B3" s="42"/>
-      <c r="C3" s="42"/>
-      <c r="D3" s="42"/>
-      <c r="E3" s="42"/>
-      <c r="F3" s="42"/>
+      <c r="A3" s="40"/>
+      <c r="B3" s="40"/>
+      <c r="C3" s="40"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="40"/>
     </row>
     <row r="4" spans="1:13" ht="40.049999999999997" customHeight="1">
       <c r="A4" s="6" t="s">
         <v>110</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>180</v>
+        <v>149</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>181</v>
+        <v>150</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>190</v>
+        <v>159</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>200</v>
+        <v>169</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>201</v>
-      </c>
-      <c r="G4" s="16"/>
-      <c r="H4" s="16"/>
-      <c r="I4" s="16"/>
-      <c r="J4" s="16"/>
-      <c r="K4" s="16"/>
-      <c r="L4" s="16"/>
-      <c r="M4" s="16"/>
+        <v>170</v>
+      </c>
+      <c r="G4" s="15"/>
+      <c r="H4" s="15"/>
+      <c r="I4" s="15"/>
+      <c r="J4" s="15"/>
+      <c r="K4" s="15"/>
+      <c r="L4" s="15"/>
+      <c r="M4" s="15"/>
     </row>
     <row r="5" spans="1:13" ht="40.049999999999997" customHeight="1">
-      <c r="A5" s="39" t="s">
+      <c r="A5" s="38" t="s">
         <v>118</v>
       </c>
-      <c r="B5" s="40" t="s">
+      <c r="B5" s="39" t="s">
+        <v>143</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>151</v>
+      </c>
+      <c r="D5" s="17" t="s">
+        <v>245</v>
+      </c>
+      <c r="E5" s="41" t="s">
+        <v>171</v>
+      </c>
+      <c r="F5" s="39" t="s">
+        <v>246</v>
+      </c>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
+      <c r="I5" s="15"/>
+      <c r="J5" s="15"/>
+      <c r="K5" s="15"/>
+      <c r="L5" s="15"/>
+      <c r="M5" s="15"/>
+    </row>
+    <row r="6" spans="1:13" ht="40.049999999999997" customHeight="1">
+      <c r="A6" s="38"/>
+      <c r="B6" s="39"/>
+      <c r="C6" s="36" t="s">
+        <v>247</v>
+      </c>
+      <c r="D6" s="17" t="s">
+        <v>248</v>
+      </c>
+      <c r="E6" s="41"/>
+      <c r="F6" s="39"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="15"/>
+      <c r="L6" s="15"/>
+      <c r="M6" s="15"/>
+    </row>
+    <row r="7" spans="1:13" ht="40.049999999999997" customHeight="1">
+      <c r="A7" s="38"/>
+      <c r="B7" s="39"/>
+      <c r="C7" s="37"/>
+      <c r="D7" s="17" t="s">
         <v>160</v>
       </c>
-      <c r="C5" s="18" t="s">
-        <v>182</v>
-      </c>
-      <c r="D5" s="18" t="s">
-        <v>276</v>
-      </c>
-      <c r="E5" s="41" t="s">
-        <v>202</v>
-      </c>
-      <c r="F5" s="40" t="s">
-        <v>277</v>
-      </c>
-      <c r="G5" s="16"/>
-      <c r="H5" s="16"/>
-      <c r="I5" s="16"/>
-      <c r="J5" s="16"/>
-      <c r="K5" s="16"/>
-      <c r="L5" s="16"/>
-      <c r="M5" s="16"/>
-    </row>
-    <row r="6" spans="1:13" ht="40.049999999999997" customHeight="1">
-      <c r="A6" s="39"/>
-      <c r="B6" s="40"/>
-      <c r="C6" s="35" t="s">
-        <v>278</v>
-      </c>
-      <c r="D6" s="18" t="s">
-        <v>279</v>
-      </c>
-      <c r="E6" s="41"/>
-      <c r="F6" s="40"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="16"/>
-      <c r="I6" s="16"/>
-      <c r="J6" s="16"/>
-      <c r="K6" s="16"/>
-      <c r="L6" s="16"/>
-      <c r="M6" s="16"/>
-    </row>
-    <row r="7" spans="1:13" ht="40.049999999999997" customHeight="1">
-      <c r="A7" s="39"/>
-      <c r="B7" s="40"/>
-      <c r="C7" s="36"/>
-      <c r="D7" s="18" t="s">
-        <v>191</v>
-      </c>
       <c r="E7" s="41"/>
-      <c r="F7" s="40"/>
-      <c r="G7" s="16"/>
-      <c r="H7" s="16"/>
-      <c r="I7" s="16"/>
-      <c r="J7" s="16"/>
-      <c r="K7" s="16"/>
-      <c r="L7" s="16"/>
-      <c r="M7" s="16"/>
+      <c r="F7" s="39"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="15"/>
+      <c r="K7" s="15"/>
+      <c r="L7" s="15"/>
+      <c r="M7" s="15"/>
     </row>
     <row r="8" spans="1:13" ht="40.049999999999997" customHeight="1">
-      <c r="A8" s="39" t="s">
+      <c r="A8" s="38" t="s">
         <v>119</v>
       </c>
-      <c r="B8" s="40" t="s">
-        <v>183</v>
-      </c>
-      <c r="C8" s="18" t="s">
-        <v>184</v>
-      </c>
-      <c r="D8" s="18" t="s">
-        <v>280</v>
+      <c r="B8" s="39" t="s">
+        <v>152</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>153</v>
+      </c>
+      <c r="D8" s="17" t="s">
+        <v>249</v>
       </c>
       <c r="E8" s="41" t="s">
-        <v>202</v>
-      </c>
-      <c r="F8" s="40" t="s">
-        <v>203</v>
-      </c>
-      <c r="G8" s="16"/>
-      <c r="H8" s="16"/>
-      <c r="I8" s="16"/>
-      <c r="J8" s="16"/>
-      <c r="K8" s="16"/>
-      <c r="L8" s="16"/>
-      <c r="M8" s="16"/>
+        <v>171</v>
+      </c>
+      <c r="F8" s="39" t="s">
+        <v>172</v>
+      </c>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="15"/>
+      <c r="J8" s="15"/>
+      <c r="K8" s="15"/>
+      <c r="L8" s="15"/>
+      <c r="M8" s="15"/>
     </row>
     <row r="9" spans="1:13" ht="40.049999999999997" customHeight="1">
-      <c r="A9" s="39"/>
-      <c r="B9" s="40"/>
-      <c r="C9" s="35" t="s">
-        <v>281</v>
-      </c>
-      <c r="D9" s="18" t="s">
-        <v>192</v>
+      <c r="A9" s="38"/>
+      <c r="B9" s="39"/>
+      <c r="C9" s="36" t="s">
+        <v>250</v>
+      </c>
+      <c r="D9" s="17" t="s">
+        <v>161</v>
       </c>
       <c r="E9" s="41"/>
-      <c r="F9" s="40"/>
-      <c r="G9" s="16"/>
-      <c r="H9" s="16"/>
-      <c r="I9" s="16"/>
-      <c r="J9" s="16"/>
-      <c r="K9" s="16"/>
-      <c r="L9" s="16"/>
-      <c r="M9" s="16"/>
+      <c r="F9" s="39"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="15"/>
+      <c r="K9" s="15"/>
+      <c r="L9" s="15"/>
+      <c r="M9" s="15"/>
     </row>
     <row r="10" spans="1:13" ht="40.049999999999997" customHeight="1">
-      <c r="A10" s="39"/>
-      <c r="B10" s="40"/>
-      <c r="C10" s="36"/>
-      <c r="D10" s="18" t="s">
-        <v>193</v>
+      <c r="A10" s="38"/>
+      <c r="B10" s="39"/>
+      <c r="C10" s="37"/>
+      <c r="D10" s="17" t="s">
+        <v>162</v>
       </c>
       <c r="E10" s="41"/>
-      <c r="F10" s="40"/>
-      <c r="G10" s="16"/>
-      <c r="H10" s="16"/>
-      <c r="I10" s="16"/>
-      <c r="J10" s="16"/>
-      <c r="K10" s="16"/>
-      <c r="L10" s="16"/>
-      <c r="M10" s="16"/>
+      <c r="F10" s="39"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="15"/>
+      <c r="J10" s="15"/>
+      <c r="K10" s="15"/>
+      <c r="L10" s="15"/>
+      <c r="M10" s="15"/>
     </row>
     <row r="11" spans="1:13" ht="40.049999999999997" customHeight="1">
-      <c r="A11" s="39" t="s">
+      <c r="A11" s="38" t="s">
         <v>120</v>
       </c>
-      <c r="B11" s="40" t="s">
-        <v>162</v>
-      </c>
-      <c r="C11" s="18" t="s">
-        <v>185</v>
-      </c>
-      <c r="D11" s="18" t="s">
-        <v>282</v>
+      <c r="B11" s="39" t="s">
+        <v>144</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>154</v>
+      </c>
+      <c r="D11" s="17" t="s">
+        <v>251</v>
       </c>
       <c r="E11" s="41" t="s">
-        <v>202</v>
-      </c>
-      <c r="F11" s="40" t="s">
-        <v>283</v>
-      </c>
-      <c r="G11" s="16"/>
-      <c r="H11" s="16"/>
-      <c r="I11" s="16"/>
-      <c r="J11" s="16"/>
-      <c r="K11" s="16"/>
-      <c r="L11" s="16"/>
-      <c r="M11" s="16"/>
+        <v>171</v>
+      </c>
+      <c r="F11" s="39" t="s">
+        <v>252</v>
+      </c>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="15"/>
+      <c r="J11" s="15"/>
+      <c r="K11" s="15"/>
+      <c r="L11" s="15"/>
+      <c r="M11" s="15"/>
     </row>
     <row r="12" spans="1:13" ht="40.049999999999997" customHeight="1">
-      <c r="A12" s="39"/>
-      <c r="B12" s="40"/>
-      <c r="C12" s="35" t="s">
-        <v>284</v>
-      </c>
-      <c r="D12" s="18" t="s">
-        <v>194</v>
+      <c r="A12" s="38"/>
+      <c r="B12" s="39"/>
+      <c r="C12" s="36" t="s">
+        <v>253</v>
+      </c>
+      <c r="D12" s="17" t="s">
+        <v>163</v>
       </c>
       <c r="E12" s="41"/>
-      <c r="F12" s="40"/>
-      <c r="G12" s="16"/>
-      <c r="H12" s="16"/>
-      <c r="I12" s="16"/>
-      <c r="J12" s="16"/>
-      <c r="K12" s="16"/>
-      <c r="L12" s="16"/>
-      <c r="M12" s="16"/>
+      <c r="F12" s="39"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="15"/>
+      <c r="I12" s="15"/>
+      <c r="J12" s="15"/>
+      <c r="K12" s="15"/>
+      <c r="L12" s="15"/>
+      <c r="M12" s="15"/>
     </row>
     <row r="13" spans="1:13" ht="40.049999999999997" customHeight="1">
-      <c r="A13" s="39"/>
-      <c r="B13" s="40"/>
-      <c r="C13" s="36"/>
-      <c r="D13" s="18" t="s">
-        <v>195</v>
+      <c r="A13" s="38"/>
+      <c r="B13" s="39"/>
+      <c r="C13" s="37"/>
+      <c r="D13" s="17" t="s">
+        <v>164</v>
       </c>
       <c r="E13" s="41"/>
-      <c r="F13" s="40"/>
-      <c r="G13" s="16"/>
-      <c r="H13" s="16"/>
-      <c r="I13" s="16"/>
-      <c r="J13" s="16"/>
-      <c r="K13" s="16"/>
-      <c r="L13" s="16"/>
-      <c r="M13" s="16"/>
+      <c r="F13" s="39"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="15"/>
+      <c r="I13" s="15"/>
+      <c r="J13" s="15"/>
+      <c r="K13" s="15"/>
+      <c r="L13" s="15"/>
+      <c r="M13" s="15"/>
     </row>
     <row r="14" spans="1:13" ht="40.049999999999997" customHeight="1">
-      <c r="A14" s="39" t="s">
+      <c r="A14" s="38" t="s">
         <v>121</v>
       </c>
-      <c r="B14" s="40" t="s">
-        <v>163</v>
-      </c>
-      <c r="C14" s="18" t="s">
-        <v>186</v>
-      </c>
-      <c r="D14" s="18" t="s">
-        <v>285</v>
+      <c r="B14" s="39" t="s">
+        <v>145</v>
+      </c>
+      <c r="C14" s="17" t="s">
+        <v>155</v>
+      </c>
+      <c r="D14" s="17" t="s">
+        <v>254</v>
       </c>
       <c r="E14" s="41" t="s">
-        <v>204</v>
-      </c>
-      <c r="F14" s="40" t="s">
-        <v>205</v>
-      </c>
-      <c r="G14" s="16"/>
-      <c r="H14" s="16"/>
-      <c r="I14" s="16"/>
-      <c r="J14" s="16"/>
-      <c r="K14" s="16"/>
-      <c r="L14" s="16"/>
-      <c r="M14" s="16"/>
+        <v>173</v>
+      </c>
+      <c r="F14" s="39" t="s">
+        <v>174</v>
+      </c>
+      <c r="G14" s="15"/>
+      <c r="H14" s="15"/>
+      <c r="I14" s="15"/>
+      <c r="J14" s="15"/>
+      <c r="K14" s="15"/>
+      <c r="L14" s="15"/>
+      <c r="M14" s="15"/>
     </row>
     <row r="15" spans="1:13" ht="40.049999999999997" customHeight="1">
-      <c r="A15" s="39"/>
-      <c r="B15" s="40"/>
-      <c r="C15" s="35" t="s">
-        <v>286</v>
-      </c>
-      <c r="D15" s="18" t="s">
-        <v>196</v>
+      <c r="A15" s="38"/>
+      <c r="B15" s="39"/>
+      <c r="C15" s="36" t="s">
+        <v>255</v>
+      </c>
+      <c r="D15" s="17" t="s">
+        <v>165</v>
       </c>
       <c r="E15" s="41"/>
-      <c r="F15" s="40"/>
-      <c r="G15" s="16"/>
-      <c r="H15" s="16"/>
-      <c r="I15" s="16"/>
-      <c r="J15" s="16"/>
-      <c r="K15" s="16"/>
-      <c r="L15" s="16"/>
-      <c r="M15" s="16"/>
+      <c r="F15" s="39"/>
+      <c r="G15" s="15"/>
+      <c r="H15" s="15"/>
+      <c r="I15" s="15"/>
+      <c r="J15" s="15"/>
+      <c r="K15" s="15"/>
+      <c r="L15" s="15"/>
+      <c r="M15" s="15"/>
     </row>
     <row r="16" spans="1:13" ht="40.049999999999997" customHeight="1">
-      <c r="A16" s="39"/>
-      <c r="B16" s="40"/>
-      <c r="C16" s="36"/>
-      <c r="D16" s="18" t="s">
-        <v>197</v>
+      <c r="A16" s="38"/>
+      <c r="B16" s="39"/>
+      <c r="C16" s="37"/>
+      <c r="D16" s="17" t="s">
+        <v>166</v>
       </c>
       <c r="E16" s="41"/>
-      <c r="F16" s="40"/>
-      <c r="G16" s="16"/>
-      <c r="H16" s="16"/>
-      <c r="I16" s="16"/>
-      <c r="J16" s="16"/>
-      <c r="K16" s="16"/>
-      <c r="L16" s="16"/>
-      <c r="M16" s="16"/>
+      <c r="F16" s="39"/>
+      <c r="G16" s="15"/>
+      <c r="H16" s="15"/>
+      <c r="I16" s="15"/>
+      <c r="J16" s="15"/>
+      <c r="K16" s="15"/>
+      <c r="L16" s="15"/>
+      <c r="M16" s="15"/>
     </row>
     <row r="17" spans="1:13" ht="40.049999999999997" customHeight="1">
-      <c r="A17" s="39" t="s">
+      <c r="A17" s="38" t="s">
         <v>122</v>
       </c>
-      <c r="B17" s="40" t="s">
-        <v>164</v>
-      </c>
-      <c r="C17" s="18" t="s">
-        <v>187</v>
-      </c>
-      <c r="D17" s="18" t="s">
-        <v>287</v>
+      <c r="B17" s="39" t="s">
+        <v>146</v>
+      </c>
+      <c r="C17" s="17" t="s">
+        <v>156</v>
+      </c>
+      <c r="D17" s="17" t="s">
+        <v>256</v>
       </c>
       <c r="E17" s="41" t="s">
-        <v>202</v>
-      </c>
-      <c r="F17" s="40" t="s">
-        <v>206</v>
-      </c>
-      <c r="G17" s="16"/>
-      <c r="H17" s="16"/>
-      <c r="I17" s="16"/>
-      <c r="J17" s="16"/>
-      <c r="K17" s="16"/>
-      <c r="L17" s="16"/>
-      <c r="M17" s="16"/>
+        <v>171</v>
+      </c>
+      <c r="F17" s="39" t="s">
+        <v>175</v>
+      </c>
+      <c r="G17" s="15"/>
+      <c r="H17" s="15"/>
+      <c r="I17" s="15"/>
+      <c r="J17" s="15"/>
+      <c r="K17" s="15"/>
+      <c r="L17" s="15"/>
+      <c r="M17" s="15"/>
     </row>
     <row r="18" spans="1:13" ht="40.049999999999997" customHeight="1">
-      <c r="A18" s="39"/>
-      <c r="B18" s="40"/>
-      <c r="C18" s="35" t="s">
-        <v>288</v>
-      </c>
-      <c r="D18" s="37" t="s">
-        <v>198</v>
+      <c r="A18" s="38"/>
+      <c r="B18" s="39"/>
+      <c r="C18" s="36" t="s">
+        <v>257</v>
+      </c>
+      <c r="D18" s="42" t="s">
+        <v>167</v>
       </c>
       <c r="E18" s="41"/>
-      <c r="F18" s="40"/>
-      <c r="G18" s="16"/>
-      <c r="H18" s="16"/>
-      <c r="I18" s="16"/>
-      <c r="J18" s="16"/>
-      <c r="K18" s="16"/>
-      <c r="L18" s="16"/>
-      <c r="M18" s="16"/>
+      <c r="F18" s="39"/>
+      <c r="G18" s="15"/>
+      <c r="H18" s="15"/>
+      <c r="I18" s="15"/>
+      <c r="J18" s="15"/>
+      <c r="K18" s="15"/>
+      <c r="L18" s="15"/>
+      <c r="M18" s="15"/>
     </row>
     <row r="19" spans="1:13" ht="40.049999999999997" customHeight="1">
-      <c r="A19" s="39"/>
-      <c r="B19" s="40"/>
-      <c r="C19" s="36"/>
-      <c r="D19" s="38"/>
+      <c r="A19" s="38"/>
+      <c r="B19" s="39"/>
+      <c r="C19" s="37"/>
+      <c r="D19" s="43"/>
       <c r="E19" s="41"/>
-      <c r="F19" s="40"/>
-      <c r="G19" s="16"/>
-      <c r="H19" s="16"/>
-      <c r="I19" s="16"/>
-      <c r="J19" s="16"/>
-      <c r="K19" s="16"/>
-      <c r="L19" s="16"/>
-      <c r="M19" s="16"/>
+      <c r="F19" s="39"/>
+      <c r="G19" s="15"/>
+      <c r="H19" s="15"/>
+      <c r="I19" s="15"/>
+      <c r="J19" s="15"/>
+      <c r="K19" s="15"/>
+      <c r="L19" s="15"/>
+      <c r="M19" s="15"/>
     </row>
     <row r="20" spans="1:13" ht="40.049999999999997" customHeight="1">
-      <c r="A20" s="17" t="s">
+      <c r="A20" s="16" t="s">
         <v>123</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>188</v>
-      </c>
-      <c r="C20" s="18" t="s">
-        <v>189</v>
-      </c>
-      <c r="D20" s="18" t="s">
-        <v>199</v>
+        <v>157</v>
+      </c>
+      <c r="C20" s="17" t="s">
+        <v>158</v>
+      </c>
+      <c r="D20" s="17" t="s">
+        <v>168</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>202</v>
+        <v>171</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>207</v>
-      </c>
-      <c r="G20" s="16"/>
-      <c r="H20" s="16"/>
-      <c r="I20" s="16"/>
-      <c r="J20" s="16"/>
-      <c r="K20" s="16"/>
-      <c r="L20" s="16"/>
-      <c r="M20" s="16"/>
+        <v>176</v>
+      </c>
+      <c r="G20" s="15"/>
+      <c r="H20" s="15"/>
+      <c r="I20" s="15"/>
+      <c r="J20" s="15"/>
+      <c r="K20" s="15"/>
+      <c r="L20" s="15"/>
+      <c r="M20" s="15"/>
     </row>
     <row r="21" spans="1:13" ht="40.049999999999997" customHeight="1">
-      <c r="A21" s="42" t="s">
-        <v>275</v>
-      </c>
-      <c r="B21" s="42"/>
-      <c r="C21" s="42"/>
-      <c r="D21" s="42"/>
-      <c r="E21" s="42"/>
-      <c r="F21" s="42"/>
+      <c r="A21" s="40" t="s">
+        <v>244</v>
+      </c>
+      <c r="B21" s="40"/>
+      <c r="C21" s="40"/>
+      <c r="D21" s="40"/>
+      <c r="E21" s="40"/>
+      <c r="F21" s="40"/>
     </row>
     <row r="22" spans="1:13" ht="40.049999999999997" customHeight="1">
       <c r="A22" s="6" t="s">
         <v>110</v>
       </c>
       <c r="B22" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="F22" s="6" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" ht="40.049999999999997" customHeight="1">
+      <c r="A23" s="38" t="s">
+        <v>124</v>
+      </c>
+      <c r="B23" s="39" t="s">
+        <v>180</v>
+      </c>
+      <c r="C23" s="17" t="s">
+        <v>181</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="E23" s="41" t="s">
+        <v>171</v>
+      </c>
+      <c r="F23" s="39" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" ht="40.049999999999997" customHeight="1">
+      <c r="A24" s="38"/>
+      <c r="B24" s="39"/>
+      <c r="C24" s="17" t="s">
+        <v>182</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="E24" s="41"/>
+      <c r="F24" s="39"/>
+    </row>
+    <row r="25" spans="1:13" ht="40.049999999999997" customHeight="1">
+      <c r="A25" s="38" t="s">
+        <v>125</v>
+      </c>
+      <c r="B25" s="39" t="s">
+        <v>186</v>
+      </c>
+      <c r="C25" s="17" t="s">
+        <v>187</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="E25" s="41" t="s">
+        <v>171</v>
+      </c>
+      <c r="F25" s="39" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" ht="40.049999999999997" customHeight="1">
+      <c r="A26" s="38"/>
+      <c r="B26" s="39"/>
+      <c r="C26" s="17" t="s">
+        <v>188</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>191</v>
+      </c>
+      <c r="E26" s="41"/>
+      <c r="F26" s="39"/>
+    </row>
+    <row r="27" spans="1:13" ht="40.049999999999997" customHeight="1">
+      <c r="A27" s="38"/>
+      <c r="B27" s="39"/>
+      <c r="C27" s="17" t="s">
+        <v>189</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="E27" s="41"/>
+      <c r="F27" s="39"/>
+    </row>
+    <row r="28" spans="1:13" ht="40.049999999999997" customHeight="1">
+      <c r="A28" s="38" t="s">
+        <v>126</v>
+      </c>
+      <c r="B28" s="39" t="s">
+        <v>194</v>
+      </c>
+      <c r="C28" s="17" t="s">
+        <v>195</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="E28" s="41" t="s">
+        <v>171</v>
+      </c>
+      <c r="F28" s="39" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" ht="40.049999999999997" customHeight="1">
+      <c r="A29" s="38"/>
+      <c r="B29" s="39"/>
+      <c r="C29" s="17" t="s">
+        <v>196</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="E29" s="41"/>
+      <c r="F29" s="39"/>
+    </row>
+    <row r="30" spans="1:13" ht="40.049999999999997" customHeight="1">
+      <c r="A30" s="38" t="s">
+        <v>127</v>
+      </c>
+      <c r="B30" s="39" t="s">
+        <v>200</v>
+      </c>
+      <c r="C30" s="17" t="s">
+        <v>201</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="E30" s="41" t="s">
+        <v>173</v>
+      </c>
+      <c r="F30" s="39" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" ht="40.049999999999997" customHeight="1">
+      <c r="A31" s="38"/>
+      <c r="B31" s="39"/>
+      <c r="C31" s="42" t="s">
+        <v>202</v>
+      </c>
+      <c r="D31" s="7" t="s">
+        <v>204</v>
+      </c>
+      <c r="E31" s="41"/>
+      <c r="F31" s="39"/>
+    </row>
+    <row r="32" spans="1:13" ht="40.049999999999997" customHeight="1">
+      <c r="A32" s="38"/>
+      <c r="B32" s="39"/>
+      <c r="C32" s="43"/>
+      <c r="D32" s="7" t="s">
+        <v>205</v>
+      </c>
+      <c r="E32" s="41"/>
+      <c r="F32" s="39"/>
+    </row>
+    <row r="33" spans="1:6" ht="40.049999999999997" customHeight="1">
+      <c r="A33" s="38" t="s">
+        <v>207</v>
+      </c>
+      <c r="B33" s="39" t="s">
         <v>208</v>
       </c>
-      <c r="C22" s="6" t="s">
-        <v>181</v>
-      </c>
-      <c r="D22" s="6" t="s">
+      <c r="C33" s="17" t="s">
         <v>209</v>
       </c>
-      <c r="E22" s="6" t="s">
-        <v>200</v>
-      </c>
-      <c r="F22" s="6" t="s">
+      <c r="D33" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="E33" s="41" t="s">
+        <v>173</v>
+      </c>
+      <c r="F33" s="39" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="40.049999999999997" customHeight="1">
+      <c r="A34" s="38"/>
+      <c r="B34" s="39"/>
+      <c r="C34" s="17" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="23" spans="1:13" ht="40.049999999999997" customHeight="1">
-      <c r="A23" s="39" t="s">
-        <v>124</v>
-      </c>
-      <c r="B23" s="40" t="s">
-        <v>211</v>
-      </c>
-      <c r="C23" s="18" t="s">
+      <c r="D34" s="7" t="s">
         <v>212</v>
       </c>
-      <c r="D23" s="7" t="s">
+      <c r="E34" s="41"/>
+      <c r="F34" s="39"/>
+    </row>
+    <row r="35" spans="1:6" ht="40.049999999999997" customHeight="1">
+      <c r="A35" s="38" t="s">
         <v>214</v>
       </c>
-      <c r="E23" s="41" t="s">
-        <v>202</v>
-      </c>
-      <c r="F23" s="40" t="s">
+      <c r="B35" s="39" t="s">
+        <v>215</v>
+      </c>
+      <c r="C35" s="17" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="24" spans="1:13" ht="40.049999999999997" customHeight="1">
-      <c r="A24" s="39"/>
-      <c r="B24" s="40"/>
-      <c r="C24" s="18" t="s">
-        <v>213</v>
-      </c>
-      <c r="D24" s="7" t="s">
-        <v>215</v>
-      </c>
-      <c r="E24" s="41"/>
-      <c r="F24" s="40"/>
-    </row>
-    <row r="25" spans="1:13" ht="40.049999999999997" customHeight="1">
-      <c r="A25" s="39" t="s">
-        <v>125</v>
-      </c>
-      <c r="B25" s="40" t="s">
+      <c r="D35" s="7" t="s">
+        <v>218</v>
+      </c>
+      <c r="E35" s="41" t="s">
+        <v>171</v>
+      </c>
+      <c r="F35" s="39" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="40.049999999999997" customHeight="1">
+      <c r="A36" s="38"/>
+      <c r="B36" s="39"/>
+      <c r="C36" s="42" t="s">
         <v>217</v>
       </c>
-      <c r="C25" s="18" t="s">
-        <v>218</v>
-      </c>
-      <c r="D25" s="7" t="s">
-        <v>221</v>
-      </c>
-      <c r="E25" s="41" t="s">
-        <v>202</v>
-      </c>
-      <c r="F25" s="40" t="s">
+      <c r="D36" s="7" t="s">
+        <v>219</v>
+      </c>
+      <c r="E36" s="41"/>
+      <c r="F36" s="39"/>
+    </row>
+    <row r="37" spans="1:6" ht="40.049999999999997" customHeight="1">
+      <c r="A37" s="38"/>
+      <c r="B37" s="39"/>
+      <c r="C37" s="43"/>
+      <c r="D37" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="E37" s="41"/>
+      <c r="F37" s="39"/>
+    </row>
+    <row r="38" spans="1:6" ht="40.049999999999997" customHeight="1">
+      <c r="A38" s="38" t="s">
+        <v>222</v>
+      </c>
+      <c r="B38" s="39" t="s">
+        <v>223</v>
+      </c>
+      <c r="C38" s="17" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="26" spans="1:13" ht="40.049999999999997" customHeight="1">
-      <c r="A26" s="39"/>
-      <c r="B26" s="40"/>
-      <c r="C26" s="18" t="s">
-        <v>219</v>
-      </c>
-      <c r="D26" s="7" t="s">
-        <v>222</v>
-      </c>
-      <c r="E26" s="41"/>
-      <c r="F26" s="40"/>
-    </row>
-    <row r="27" spans="1:13" ht="40.049999999999997" customHeight="1">
-      <c r="A27" s="39"/>
-      <c r="B27" s="40"/>
-      <c r="C27" s="18" t="s">
-        <v>220</v>
-      </c>
-      <c r="D27" s="7" t="s">
-        <v>223</v>
-      </c>
-      <c r="E27" s="41"/>
-      <c r="F27" s="40"/>
-    </row>
-    <row r="28" spans="1:13" ht="40.049999999999997" customHeight="1">
-      <c r="A28" s="39" t="s">
-        <v>126</v>
-      </c>
-      <c r="B28" s="40" t="s">
+      <c r="D38" s="7" t="s">
+        <v>226</v>
+      </c>
+      <c r="E38" s="41" t="s">
+        <v>171</v>
+      </c>
+      <c r="F38" s="39" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="40.049999999999997" customHeight="1">
+      <c r="A39" s="38"/>
+      <c r="B39" s="39"/>
+      <c r="C39" s="17" t="s">
         <v>225</v>
       </c>
-      <c r="C28" s="18" t="s">
-        <v>226</v>
-      </c>
-      <c r="D28" s="7" t="s">
-        <v>228</v>
-      </c>
-      <c r="E28" s="41" t="s">
-        <v>202</v>
-      </c>
-      <c r="F28" s="40" t="s">
+      <c r="D39" s="7" t="s">
+        <v>227</v>
+      </c>
+      <c r="E39" s="41"/>
+      <c r="F39" s="39"/>
+    </row>
+    <row r="40" spans="1:6" ht="40.049999999999997" customHeight="1">
+      <c r="A40" s="38" t="s">
+        <v>229</v>
+      </c>
+      <c r="B40" s="39" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="29" spans="1:13" ht="40.049999999999997" customHeight="1">
-      <c r="A29" s="39"/>
-      <c r="B29" s="40"/>
-      <c r="C29" s="18" t="s">
-        <v>227</v>
-      </c>
-      <c r="D29" s="7" t="s">
-        <v>229</v>
-      </c>
-      <c r="E29" s="41"/>
-      <c r="F29" s="40"/>
-    </row>
-    <row r="30" spans="1:13" ht="40.049999999999997" customHeight="1">
-      <c r="A30" s="39" t="s">
-        <v>127</v>
-      </c>
-      <c r="B30" s="40" t="s">
+      <c r="C40" s="17" t="s">
         <v>231</v>
       </c>
-      <c r="C30" s="18" t="s">
+      <c r="D40" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="E40" s="41" t="s">
+        <v>173</v>
+      </c>
+      <c r="F40" s="39" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="40.049999999999997" customHeight="1">
+      <c r="A41" s="38"/>
+      <c r="B41" s="39"/>
+      <c r="C41" s="42" t="s">
         <v>232</v>
       </c>
-      <c r="D30" s="7" t="s">
+      <c r="D41" s="7" t="s">
         <v>234</v>
       </c>
-      <c r="E30" s="41" t="s">
-        <v>204</v>
-      </c>
-      <c r="F30" s="40" t="s">
+      <c r="E41" s="41"/>
+      <c r="F41" s="39"/>
+    </row>
+    <row r="42" spans="1:6" ht="40.049999999999997" customHeight="1">
+      <c r="A42" s="38"/>
+      <c r="B42" s="39"/>
+      <c r="C42" s="43"/>
+      <c r="D42" s="7" t="s">
+        <v>235</v>
+      </c>
+      <c r="E42" s="41"/>
+      <c r="F42" s="39"/>
+    </row>
+    <row r="43" spans="1:6" ht="40.049999999999997" customHeight="1">
+      <c r="A43" s="38" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="31" spans="1:13" ht="40.049999999999997" customHeight="1">
-      <c r="A31" s="39"/>
-      <c r="B31" s="40"/>
-      <c r="C31" s="37" t="s">
-        <v>233</v>
-      </c>
-      <c r="D31" s="7" t="s">
-        <v>235</v>
-      </c>
-      <c r="E31" s="41"/>
-      <c r="F31" s="40"/>
-    </row>
-    <row r="32" spans="1:13" ht="40.049999999999997" customHeight="1">
-      <c r="A32" s="39"/>
-      <c r="B32" s="40"/>
-      <c r="C32" s="38"/>
-      <c r="D32" s="7" t="s">
-        <v>236</v>
-      </c>
-      <c r="E32" s="41"/>
-      <c r="F32" s="40"/>
-    </row>
-    <row r="33" spans="1:6" ht="40.049999999999997" customHeight="1">
-      <c r="A33" s="39" t="s">
+      <c r="B43" s="39" t="s">
         <v>238</v>
       </c>
-      <c r="B33" s="40" t="s">
+      <c r="C43" s="17" t="s">
         <v>239</v>
       </c>
-      <c r="C33" s="18" t="s">
+      <c r="D43" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="E43" s="41" t="s">
+        <v>171</v>
+      </c>
+      <c r="F43" s="39" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="40.049999999999997" customHeight="1">
+      <c r="A44" s="38"/>
+      <c r="B44" s="39"/>
+      <c r="C44" s="17" t="s">
         <v>240</v>
       </c>
-      <c r="D33" s="7" t="s">
+      <c r="D44" s="7" t="s">
         <v>242</v>
       </c>
-      <c r="E33" s="41" t="s">
-        <v>204</v>
-      </c>
-      <c r="F33" s="40" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" ht="40.049999999999997" customHeight="1">
-      <c r="A34" s="39"/>
-      <c r="B34" s="40"/>
-      <c r="C34" s="18" t="s">
-        <v>241</v>
-      </c>
-      <c r="D34" s="7" t="s">
-        <v>243</v>
-      </c>
-      <c r="E34" s="41"/>
-      <c r="F34" s="40"/>
-    </row>
-    <row r="35" spans="1:6" ht="40.049999999999997" customHeight="1">
-      <c r="A35" s="39" t="s">
-        <v>245</v>
-      </c>
-      <c r="B35" s="40" t="s">
-        <v>246</v>
-      </c>
-      <c r="C35" s="18" t="s">
-        <v>247</v>
-      </c>
-      <c r="D35" s="7" t="s">
-        <v>249</v>
-      </c>
-      <c r="E35" s="41" t="s">
-        <v>202</v>
-      </c>
-      <c r="F35" s="40" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" ht="40.049999999999997" customHeight="1">
-      <c r="A36" s="39"/>
-      <c r="B36" s="40"/>
-      <c r="C36" s="37" t="s">
-        <v>248</v>
-      </c>
-      <c r="D36" s="7" t="s">
-        <v>250</v>
-      </c>
-      <c r="E36" s="41"/>
-      <c r="F36" s="40"/>
-    </row>
-    <row r="37" spans="1:6" ht="40.049999999999997" customHeight="1">
-      <c r="A37" s="39"/>
-      <c r="B37" s="40"/>
-      <c r="C37" s="38"/>
-      <c r="D37" s="7" t="s">
-        <v>251</v>
-      </c>
-      <c r="E37" s="41"/>
-      <c r="F37" s="40"/>
-    </row>
-    <row r="38" spans="1:6" ht="40.049999999999997" customHeight="1">
-      <c r="A38" s="39" t="s">
-        <v>253</v>
-      </c>
-      <c r="B38" s="40" t="s">
-        <v>254</v>
-      </c>
-      <c r="C38" s="18" t="s">
-        <v>255</v>
-      </c>
-      <c r="D38" s="7" t="s">
-        <v>257</v>
-      </c>
-      <c r="E38" s="41" t="s">
-        <v>202</v>
-      </c>
-      <c r="F38" s="40" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" ht="40.049999999999997" customHeight="1">
-      <c r="A39" s="39"/>
-      <c r="B39" s="40"/>
-      <c r="C39" s="18" t="s">
-        <v>256</v>
-      </c>
-      <c r="D39" s="7" t="s">
-        <v>258</v>
-      </c>
-      <c r="E39" s="41"/>
-      <c r="F39" s="40"/>
-    </row>
-    <row r="40" spans="1:6" ht="40.049999999999997" customHeight="1">
-      <c r="A40" s="39" t="s">
-        <v>260</v>
-      </c>
-      <c r="B40" s="40" t="s">
-        <v>261</v>
-      </c>
-      <c r="C40" s="18" t="s">
-        <v>262</v>
-      </c>
-      <c r="D40" s="7" t="s">
-        <v>264</v>
-      </c>
-      <c r="E40" s="41" t="s">
-        <v>204</v>
-      </c>
-      <c r="F40" s="40" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" ht="40.049999999999997" customHeight="1">
-      <c r="A41" s="39"/>
-      <c r="B41" s="40"/>
-      <c r="C41" s="37" t="s">
-        <v>263</v>
-      </c>
-      <c r="D41" s="7" t="s">
-        <v>265</v>
-      </c>
-      <c r="E41" s="41"/>
-      <c r="F41" s="40"/>
-    </row>
-    <row r="42" spans="1:6" ht="40.049999999999997" customHeight="1">
-      <c r="A42" s="39"/>
-      <c r="B42" s="40"/>
-      <c r="C42" s="38"/>
-      <c r="D42" s="7" t="s">
-        <v>266</v>
-      </c>
-      <c r="E42" s="41"/>
-      <c r="F42" s="40"/>
-    </row>
-    <row r="43" spans="1:6" ht="40.049999999999997" customHeight="1">
-      <c r="A43" s="39" t="s">
-        <v>268</v>
-      </c>
-      <c r="B43" s="40" t="s">
-        <v>269</v>
-      </c>
-      <c r="C43" s="18" t="s">
-        <v>270</v>
-      </c>
-      <c r="D43" s="7" t="s">
-        <v>272</v>
-      </c>
-      <c r="E43" s="41" t="s">
-        <v>202</v>
-      </c>
-      <c r="F43" s="40" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" ht="40.049999999999997" customHeight="1">
-      <c r="A44" s="39"/>
-      <c r="B44" s="40"/>
-      <c r="C44" s="18" t="s">
-        <v>271</v>
-      </c>
-      <c r="D44" s="7" t="s">
-        <v>273</v>
-      </c>
       <c r="E44" s="41"/>
-      <c r="F44" s="40"/>
+      <c r="F44" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="68">
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="A2:F3"/>
-    <mergeCell ref="E5:E7"/>
-    <mergeCell ref="F5:F7"/>
-    <mergeCell ref="E8:E10"/>
-    <mergeCell ref="F8:F10"/>
-    <mergeCell ref="E11:E13"/>
-    <mergeCell ref="F11:F13"/>
-    <mergeCell ref="E14:E16"/>
-    <mergeCell ref="F14:F16"/>
-    <mergeCell ref="E17:E19"/>
-    <mergeCell ref="F17:F19"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="F23:F24"/>
-    <mergeCell ref="A21:F21"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="A14:A16"/>
-    <mergeCell ref="B14:B16"/>
-    <mergeCell ref="A17:A19"/>
-    <mergeCell ref="B17:B19"/>
-    <mergeCell ref="E25:E27"/>
-    <mergeCell ref="F25:F27"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="E28:E29"/>
-    <mergeCell ref="F28:F29"/>
-    <mergeCell ref="E30:E32"/>
-    <mergeCell ref="F30:F32"/>
-    <mergeCell ref="A33:A34"/>
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="E33:E34"/>
-    <mergeCell ref="F33:F34"/>
-    <mergeCell ref="E35:E37"/>
-    <mergeCell ref="F35:F37"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="E38:E39"/>
-    <mergeCell ref="F38:F39"/>
-    <mergeCell ref="E40:E42"/>
-    <mergeCell ref="F40:F42"/>
-    <mergeCell ref="A43:A44"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="E43:E44"/>
-    <mergeCell ref="F43:F44"/>
     <mergeCell ref="C12:C13"/>
     <mergeCell ref="C31:C32"/>
     <mergeCell ref="C36:C37"/>
@@ -4623,6 +4172,60 @@
     <mergeCell ref="B25:B27"/>
     <mergeCell ref="A11:A13"/>
     <mergeCell ref="B11:B13"/>
+    <mergeCell ref="E40:E42"/>
+    <mergeCell ref="F40:F42"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="E43:E44"/>
+    <mergeCell ref="F43:F44"/>
+    <mergeCell ref="E35:E37"/>
+    <mergeCell ref="F35:F37"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="E38:E39"/>
+    <mergeCell ref="F38:F39"/>
+    <mergeCell ref="E30:E32"/>
+    <mergeCell ref="F30:F32"/>
+    <mergeCell ref="A33:A34"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="E33:E34"/>
+    <mergeCell ref="F33:F34"/>
+    <mergeCell ref="E25:E27"/>
+    <mergeCell ref="F25:F27"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="E28:E29"/>
+    <mergeCell ref="F28:F29"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="F23:F24"/>
+    <mergeCell ref="A21:F21"/>
+    <mergeCell ref="E11:E13"/>
+    <mergeCell ref="F11:F13"/>
+    <mergeCell ref="E14:E16"/>
+    <mergeCell ref="F14:F16"/>
+    <mergeCell ref="E17:E19"/>
+    <mergeCell ref="F17:F19"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="A2:F3"/>
+    <mergeCell ref="E5:E7"/>
+    <mergeCell ref="F5:F7"/>
+    <mergeCell ref="E8:E10"/>
+    <mergeCell ref="F8:F10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4632,8 +4235,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE1CDD62-96F2-41A0-B21D-3547ED58FC98}">
   <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -4647,38 +4250,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="46" t="s">
-        <v>360</v>
-      </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
+      <c r="A1" s="44" t="s">
+        <v>329</v>
+      </c>
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="46"/>
-      <c r="B2" s="46"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
+      <c r="A2" s="44"/>
+      <c r="B2" s="44"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="46"/>
-      <c r="B3" s="46"/>
-      <c r="C3" s="46"/>
-      <c r="D3" s="46"/>
-      <c r="E3" s="46"/>
-      <c r="F3" s="46"/>
+      <c r="A3" s="44"/>
+      <c r="B3" s="44"/>
+      <c r="C3" s="44"/>
+      <c r="D3" s="44"/>
+      <c r="E3" s="44"/>
+      <c r="F3" s="44"/>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="47"/>
-      <c r="B4" s="47"/>
-      <c r="C4" s="47"/>
-      <c r="D4" s="47"/>
-      <c r="E4" s="47"/>
-      <c r="F4" s="47"/>
+      <c r="A4" s="45"/>
+      <c r="B4" s="45"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
     </row>
     <row r="5" spans="1:6" ht="28.8">
       <c r="A5" s="6" t="s">
@@ -4688,390 +4291,370 @@
         <v>129</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>289</v>
+        <v>258</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>290</v>
+        <v>259</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>291</v>
+        <v>260</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>325</v>
+        <v>294</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="28.8">
-      <c r="A6" s="17" t="s">
-        <v>361</v>
-      </c>
-      <c r="B6" s="17" t="s">
+      <c r="A6" s="16" t="s">
+        <v>330</v>
+      </c>
+      <c r="B6" s="16" t="s">
         <v>130</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>292</v>
+        <v>261</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>293</v>
+        <v>262</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>294</v>
+        <v>263</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>326</v>
+        <v>295</v>
       </c>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="39" t="s">
-        <v>362</v>
-      </c>
-      <c r="B7" s="39" t="s">
+      <c r="A7" s="38" t="s">
+        <v>331</v>
+      </c>
+      <c r="B7" s="38" t="s">
         <v>131</v>
       </c>
-      <c r="C7" s="40" t="s">
-        <v>295</v>
+      <c r="C7" s="39" t="s">
+        <v>264</v>
       </c>
       <c r="D7" s="7" t="s">
+        <v>265</v>
+      </c>
+      <c r="E7" s="39" t="s">
+        <v>267</v>
+      </c>
+      <c r="F7" s="39" t="s">
         <v>296</v>
       </c>
-      <c r="E7" s="40" t="s">
+    </row>
+    <row r="8" spans="1:6" ht="28.8">
+      <c r="A8" s="38"/>
+      <c r="B8" s="38"/>
+      <c r="C8" s="39"/>
+      <c r="D8" s="7" t="s">
+        <v>266</v>
+      </c>
+      <c r="E8" s="39"/>
+      <c r="F8" s="39"/>
+    </row>
+    <row r="9" spans="1:6" ht="28.8">
+      <c r="A9" s="38" t="s">
+        <v>332</v>
+      </c>
+      <c r="B9" s="38" t="s">
+        <v>132</v>
+      </c>
+      <c r="C9" s="39" t="s">
+        <v>268</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>269</v>
+      </c>
+      <c r="E9" s="39" t="s">
+        <v>133</v>
+      </c>
+      <c r="F9" s="39" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="38"/>
+      <c r="B10" s="38"/>
+      <c r="C10" s="39"/>
+      <c r="D10" s="7" t="s">
+        <v>270</v>
+      </c>
+      <c r="E10" s="39"/>
+      <c r="F10" s="39"/>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="38" t="s">
+        <v>333</v>
+      </c>
+      <c r="B11" s="38" t="s">
+        <v>134</v>
+      </c>
+      <c r="C11" s="39" t="s">
+        <v>271</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>272</v>
+      </c>
+      <c r="E11" s="39" t="s">
+        <v>135</v>
+      </c>
+      <c r="F11" s="39" t="s">
         <v>298</v>
       </c>
-      <c r="F7" s="40" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="28.8">
-      <c r="A8" s="39"/>
-      <c r="B8" s="39"/>
-      <c r="C8" s="40"/>
-      <c r="D8" s="7" t="s">
-        <v>297</v>
-      </c>
-      <c r="E8" s="40"/>
-      <c r="F8" s="40"/>
-    </row>
-    <row r="9" spans="1:6" ht="28.8">
-      <c r="A9" s="39" t="s">
-        <v>363</v>
-      </c>
-      <c r="B9" s="39" t="s">
-        <v>132</v>
-      </c>
-      <c r="C9" s="40" t="s">
+    </row>
+    <row r="12" spans="1:6" ht="28.8">
+      <c r="A12" s="38"/>
+      <c r="B12" s="38"/>
+      <c r="C12" s="39"/>
+      <c r="D12" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="E12" s="39"/>
+      <c r="F12" s="39"/>
+    </row>
+    <row r="13" spans="1:6" ht="28.8">
+      <c r="A13" s="16" t="s">
+        <v>334</v>
+      </c>
+      <c r="B13" s="16" t="s">
+        <v>274</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>275</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>276</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>277</v>
+      </c>
+      <c r="F13" s="7" t="s">
         <v>299</v>
       </c>
-      <c r="D9" s="7" t="s">
-        <v>300</v>
-      </c>
-      <c r="E9" s="40" t="s">
-        <v>133</v>
-      </c>
-      <c r="F9" s="40" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" s="39"/>
-      <c r="B10" s="39"/>
-      <c r="C10" s="40"/>
-      <c r="D10" s="7" t="s">
-        <v>301</v>
-      </c>
-      <c r="E10" s="40"/>
-      <c r="F10" s="40"/>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" s="39" t="s">
-        <v>364</v>
-      </c>
-      <c r="B11" s="39" t="s">
-        <v>134</v>
-      </c>
-      <c r="C11" s="40" t="s">
-        <v>302</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>303</v>
-      </c>
-      <c r="E11" s="40" t="s">
-        <v>135</v>
-      </c>
-      <c r="F11" s="40" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="28.8">
-      <c r="A12" s="39"/>
-      <c r="B12" s="39"/>
-      <c r="C12" s="40"/>
-      <c r="D12" s="7" t="s">
-        <v>304</v>
-      </c>
-      <c r="E12" s="40"/>
-      <c r="F12" s="40"/>
-    </row>
-    <row r="13" spans="1:6" ht="28.8">
-      <c r="A13" s="17" t="s">
-        <v>365</v>
-      </c>
-      <c r="B13" s="17" t="s">
-        <v>305</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>306</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>307</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>308</v>
-      </c>
-      <c r="F13" s="7" t="s">
-        <v>330</v>
-      </c>
     </row>
     <row r="14" spans="1:6" ht="43.2">
-      <c r="A14" s="17" t="s">
-        <v>366</v>
-      </c>
-      <c r="B14" s="17" t="s">
-        <v>309</v>
+      <c r="A14" s="16" t="s">
+        <v>335</v>
+      </c>
+      <c r="B14" s="16" t="s">
+        <v>278</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>310</v>
+        <v>279</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>311</v>
+        <v>280</v>
       </c>
       <c r="E14" s="7" t="s">
         <v>136</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>331</v>
+        <v>300</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="28.8">
-      <c r="A15" s="39" t="s">
-        <v>367</v>
-      </c>
-      <c r="B15" s="39" t="s">
+      <c r="A15" s="38" t="s">
+        <v>336</v>
+      </c>
+      <c r="B15" s="38" t="s">
+        <v>281</v>
+      </c>
+      <c r="C15" s="39" t="s">
+        <v>282</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>283</v>
+      </c>
+      <c r="E15" s="39" t="s">
+        <v>285</v>
+      </c>
+      <c r="F15" s="39" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="38"/>
+      <c r="B16" s="38"/>
+      <c r="C16" s="39"/>
+      <c r="D16" s="7" t="s">
+        <v>284</v>
+      </c>
+      <c r="E16" s="39"/>
+      <c r="F16" s="39"/>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="38" t="s">
+        <v>337</v>
+      </c>
+      <c r="B17" s="38" t="s">
+        <v>286</v>
+      </c>
+      <c r="C17" s="39" t="s">
+        <v>282</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>287</v>
+      </c>
+      <c r="E17" s="39" t="s">
+        <v>289</v>
+      </c>
+      <c r="F17" s="39" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="28.8">
+      <c r="A18" s="38"/>
+      <c r="B18" s="38"/>
+      <c r="C18" s="39"/>
+      <c r="D18" s="7" t="s">
+        <v>288</v>
+      </c>
+      <c r="E18" s="39"/>
+      <c r="F18" s="39"/>
+    </row>
+    <row r="19" spans="1:6" ht="28.8">
+      <c r="A19" s="16" t="s">
+        <v>338</v>
+      </c>
+      <c r="B19" s="16" t="s">
+        <v>290</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>291</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>292</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>293</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="38" t="s">
+        <v>339</v>
+      </c>
+      <c r="B20" s="38" t="s">
+        <v>304</v>
+      </c>
+      <c r="C20" s="39" t="s">
+        <v>305</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>306</v>
+      </c>
+      <c r="E20" s="39" t="s">
+        <v>137</v>
+      </c>
+      <c r="F20" s="39" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="28.8">
+      <c r="A21" s="38"/>
+      <c r="B21" s="38"/>
+      <c r="C21" s="39"/>
+      <c r="D21" s="7" t="s">
+        <v>307</v>
+      </c>
+      <c r="E21" s="39"/>
+      <c r="F21" s="39"/>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="38" t="s">
+        <v>340</v>
+      </c>
+      <c r="B22" s="38" t="s">
+        <v>309</v>
+      </c>
+      <c r="C22" s="39" t="s">
+        <v>310</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>311</v>
+      </c>
+      <c r="E22" s="39" t="s">
+        <v>313</v>
+      </c>
+      <c r="F22" s="39" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="28.8">
+      <c r="A23" s="38"/>
+      <c r="B23" s="38"/>
+      <c r="C23" s="39"/>
+      <c r="D23" s="7" t="s">
         <v>312</v>
       </c>
-      <c r="C15" s="40" t="s">
-        <v>313</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>314</v>
-      </c>
-      <c r="E15" s="40" t="s">
+      <c r="E23" s="39"/>
+      <c r="F23" s="39"/>
+    </row>
+    <row r="24" spans="1:6" ht="28.8">
+      <c r="A24" s="16" t="s">
+        <v>341</v>
+      </c>
+      <c r="B24" s="16" t="s">
+        <v>315</v>
+      </c>
+      <c r="C24" s="7" t="s">
         <v>316</v>
       </c>
-      <c r="F15" s="40" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="A16" s="39"/>
-      <c r="B16" s="39"/>
-      <c r="C16" s="40"/>
-      <c r="D16" s="7" t="s">
-        <v>315</v>
-      </c>
-      <c r="E16" s="40"/>
-      <c r="F16" s="40"/>
-    </row>
-    <row r="17" spans="1:6">
-      <c r="A17" s="39" t="s">
-        <v>368</v>
-      </c>
-      <c r="B17" s="39" t="s">
+      <c r="D24" s="7" t="s">
         <v>317</v>
       </c>
-      <c r="C17" s="40" t="s">
-        <v>313</v>
-      </c>
-      <c r="D17" s="7" t="s">
+      <c r="E24" s="7" t="s">
         <v>318</v>
       </c>
-      <c r="E17" s="40" t="s">
+      <c r="F24" s="7" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="28.8">
+      <c r="A25" s="16" t="s">
+        <v>342</v>
+      </c>
+      <c r="B25" s="16" t="s">
         <v>320</v>
       </c>
-      <c r="F17" s="40" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="28.8">
-      <c r="A18" s="39"/>
-      <c r="B18" s="39"/>
-      <c r="C18" s="40"/>
-      <c r="D18" s="7" t="s">
-        <v>319</v>
-      </c>
-      <c r="E18" s="40"/>
-      <c r="F18" s="40"/>
-    </row>
-    <row r="19" spans="1:6" ht="28.8">
-      <c r="A19" s="17" t="s">
-        <v>369</v>
-      </c>
-      <c r="B19" s="17" t="s">
+      <c r="C25" s="7" t="s">
         <v>321</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="D25" s="7" t="s">
         <v>322</v>
-      </c>
-      <c r="D19" s="7" t="s">
-        <v>323</v>
-      </c>
-      <c r="E19" s="7" t="s">
-        <v>324</v>
-      </c>
-      <c r="F19" s="7" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
-      <c r="A20" s="39" t="s">
-        <v>370</v>
-      </c>
-      <c r="B20" s="39" t="s">
-        <v>335</v>
-      </c>
-      <c r="C20" s="40" t="s">
-        <v>336</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>337</v>
-      </c>
-      <c r="E20" s="40" t="s">
-        <v>137</v>
-      </c>
-      <c r="F20" s="40" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="28.8">
-      <c r="A21" s="39"/>
-      <c r="B21" s="39"/>
-      <c r="C21" s="40"/>
-      <c r="D21" s="7" t="s">
-        <v>338</v>
-      </c>
-      <c r="E21" s="40"/>
-      <c r="F21" s="40"/>
-    </row>
-    <row r="22" spans="1:6">
-      <c r="A22" s="39" t="s">
-        <v>371</v>
-      </c>
-      <c r="B22" s="39" t="s">
-        <v>340</v>
-      </c>
-      <c r="C22" s="40" t="s">
-        <v>341</v>
-      </c>
-      <c r="D22" s="7" t="s">
-        <v>342</v>
-      </c>
-      <c r="E22" s="40" t="s">
-        <v>344</v>
-      </c>
-      <c r="F22" s="40" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="28.8">
-      <c r="A23" s="39"/>
-      <c r="B23" s="39"/>
-      <c r="C23" s="40"/>
-      <c r="D23" s="7" t="s">
-        <v>343</v>
-      </c>
-      <c r="E23" s="40"/>
-      <c r="F23" s="40"/>
-    </row>
-    <row r="24" spans="1:6" ht="28.8">
-      <c r="A24" s="17" t="s">
-        <v>372</v>
-      </c>
-      <c r="B24" s="17" t="s">
-        <v>346</v>
-      </c>
-      <c r="C24" s="7" t="s">
-        <v>347</v>
-      </c>
-      <c r="D24" s="7" t="s">
-        <v>348</v>
-      </c>
-      <c r="E24" s="7" t="s">
-        <v>349</v>
-      </c>
-      <c r="F24" s="7" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="28.8">
-      <c r="A25" s="17" t="s">
-        <v>373</v>
-      </c>
-      <c r="B25" s="17" t="s">
-        <v>351</v>
-      </c>
-      <c r="C25" s="7" t="s">
-        <v>352</v>
-      </c>
-      <c r="D25" s="7" t="s">
-        <v>353</v>
       </c>
       <c r="E25" s="7" t="s">
         <v>138</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>354</v>
+        <v>323</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="28.8">
-      <c r="A26" s="17" t="s">
-        <v>374</v>
-      </c>
-      <c r="B26" s="17" t="s">
-        <v>355</v>
+      <c r="A26" s="16" t="s">
+        <v>343</v>
+      </c>
+      <c r="B26" s="16" t="s">
+        <v>324</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>356</v>
+        <v>325</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>357</v>
+        <v>326</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>358</v>
+        <v>327</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>359</v>
+        <v>328</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="E22:E23"/>
-    <mergeCell ref="F22:F23"/>
     <mergeCell ref="A1:F4"/>
     <mergeCell ref="A20:A21"/>
     <mergeCell ref="B20:B21"/>
@@ -5088,6 +4671,26 @@
     <mergeCell ref="F15:F16"/>
     <mergeCell ref="F17:F18"/>
     <mergeCell ref="A11:A12"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="F22:F23"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="E9:E10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>